<commit_message>
modification of objective functions facilitating finding global minima
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -414,11 +414,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>12:36:00</t>
+          <t>14:02:00</t>
         </is>
       </c>
       <c r="C2">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
added advanced forecast option
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -414,11 +414,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>14:02:00</t>
+          <t>19:23:00</t>
         </is>
       </c>
       <c r="C2">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
added calculation of AUC_24h
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -409,12 +409,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2019-12-15</t>
+          <t>2019-12-16</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>19:23:00</t>
+          <t>18:01:00</t>
         </is>
       </c>
       <c r="C2">
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>0.85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Using R2Jags instead of rjags for Gibbs-Sampling
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -353,7 +353,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -409,12 +409,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2020-01-19</t>
+          <t>2019-12-15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>07:23:00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -454,12 +454,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2020-01-20</t>
+          <t>2019-12-15</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>01:45:00</t>
+          <t>12:10:00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -469,7 +469,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E3">
@@ -491,6 +491,231 @@
         </is>
       </c>
       <c r="I3" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2019-12-15</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>18:10:00</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2019-12-15</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>19:09:00</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2019-12-16</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>06:25:00</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2019-12-16</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>07:10:00</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2019-12-16</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>12:35:00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
         <is>
           <t>.</t>
         </is>
@@ -538,10 +763,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C2">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -579,7 +804,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.85</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected a bug in the error model
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -353,7 +353,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -459,25 +459,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>12:10:00</t>
+          <t>19:09:00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>.</t>
         </is>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>60</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -499,12 +499,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2019-12-15</t>
+          <t>2019-12-16</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>18:10:00</t>
+          <t>06:25:00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -514,7 +514,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E4">
@@ -544,12 +544,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2019-12-15</t>
+          <t>2019-12-16</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>19:09:00</t>
+          <t>07:10:00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -581,141 +581,6 @@
         </is>
       </c>
       <c r="I5" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2019-12-16</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>06:25:00</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2019-12-16</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>07:10:00</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2019-12-16</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>12:35:00</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
         <is>
           <t>.</t>
         </is>
@@ -766,7 +631,7 @@
         <v>65</v>
       </c>
       <c r="C2">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="D2">
         <v>0</v>

</xml_diff>

<commit_message>
correction of error model
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -409,12 +409,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2020-01-29</t>
+          <t>2020-03-03</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10:47:00</t>
+          <t>09:32:00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -454,12 +454,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2020-01-29</t>
+          <t>2020-03-03</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>15:47:00</t>
+          <t>14:32:00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">

</xml_diff>